<commit_message>
ajustes planilha de uat
</commit_message>
<xml_diff>
--- a/Planilha_UAT_ACOLHE-SP.01.xlsx
+++ b/Planilha_UAT_ACOLHE-SP.01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/luan_collyns_s_silva_accenture_com/Documents/Documents/Anotações - TQ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victoria.a.camargo\Documents\faculdade\3 Semestre\Git\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F1CBEAC-6635-41A4-9FD6-2E8F6C2182C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308D0E6B-AB8E-4F07-80E0-6D6E32080DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="1000" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="1000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cenário - Cadastro DOADOR" sheetId="14" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="347">
   <si>
     <t>Data de homologação:</t>
   </si>
@@ -1515,10 +1515,6 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -1568,6 +1564,10 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1591,6 +1591,2534 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>577272</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>464615</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3780559</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1987857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7BD54D6-E2FD-4CDD-BB8D-9D002D5A5D49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15447817" y="4678706"/>
+          <a:ext cx="3209637" cy="1529592"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>415636</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>554182</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3724156</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>1474979</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD953C1F-B765-4CB8-9747-5EC8B0F1204D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15309272" y="7204364"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>450273</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>467591</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3755618</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1391563</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C55FF3A3-291F-4616-A9E4-4937451DE12E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15343909" y="9040091"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>519545</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>536864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3818540</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>1454486</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C944494A-BFB1-449F-AB54-D5F7BCA915F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15413181" y="10841182"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>398318</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>536864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3706838</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1457661</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44E9D609-F816-45C1-83DE-C9D62991439C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15291954" y="12798137"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>519546</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>467591</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3821716</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1391563</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{820901D1-DAC2-4025-968B-FCE578CCD304}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15413182" y="14460682"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>557356</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>481734</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3856351</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1412056</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8E62A60-1C49-47B2-8B2D-A5992986626C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15450992" y="16154689"/>
+          <a:ext cx="3302170" cy="930322"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>502228</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>519545</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3807573</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1440342</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0687AAB-1323-47F6-8A13-056BF959C516}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15395864" y="18028227"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>484910</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>450272</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3790255</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1374244</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76AFEF37-AAC4-45E5-A412-5F7D3C76B6FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15378546" y="19690772"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>675409</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>484909</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3980754</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1408881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7487B911-CABE-469A-8D0D-D7D1DA7FFDCA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15569045" y="21699682"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>554182</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>415637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3856352</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>1342784</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAABF9EB-7179-4A31-B6B3-68DC8584C694}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15447818" y="23570046"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>606136</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>346364</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3917831</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1263986</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{919F0116-C356-4B97-ACEE-A4D557C52F3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15499772" y="25319182"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>415637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3876845</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1345959</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9B4F1EE-B38C-4E0B-90E6-9512F2CCA2F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15465136" y="27362728"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>588819</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>311727</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3894164</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1235699</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A80CF042-CEBB-4196-96AF-323BE2F02DC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15482455" y="29129182"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>519545</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>484909</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3818540</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>1408881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D85C6CCF-B8C2-4265-9E69-EB55A3FE110E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15413181" y="30861000"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>467591</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>415637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3772936</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>1345959</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C9807AD-93A8-46DF-BF3C-0DA0F8C0EFF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15361227" y="32575501"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>432954</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3744649</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>1304972</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F2D39B2-AF47-4BB4-A527-9BABE824EAC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15326590" y="34411227"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>554182</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>294409</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3859527</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>1218381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8201B3C7-E9B5-4621-B3B8-66FB04CEB5F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15447818" y="35952545"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3876845</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>1304972</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66593422-02D2-49A0-92F3-F19A9FB83B48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15465136" y="37667045"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>550718</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>273627</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3856063</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>1197599</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1DCF4AB-8E4C-4332-80D0-8BA2FD997377}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15444354" y="39135627"/>
+          <a:ext cx="3305345" cy="923972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>330200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3438694</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1270048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEA59463-5E76-482A-AE91-AB1EE5C3C1C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17106900" y="5765800"/>
+          <a:ext cx="3286294" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3422819</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>1206548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69874D8B-8BE7-436E-93E9-476B4AE55360}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17094200" y="7442200"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>457200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3435519</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1397048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2030692C-D590-4CB8-8563-4DBFE913C31F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17106900" y="9194800"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>431800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3410119</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>1371648</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3425C2BF-E7F4-4B8A-9E8F-E97F2A4C748B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17081500" y="10845800"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3460919</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1219248</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4F5720C-ABA4-4EA7-A5BF-0F9FCC8CA9F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17132300" y="12357100"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3422819</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1295448</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA8B71D3-E37E-4878-8EA8-FCE795CD383F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17094200" y="13830300"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>393700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3359319</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1333548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{660F4546-CF86-4BB8-B8B1-589AFDD122B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17030700" y="15417800"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>393700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3410119</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1333548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FF7742A-C97B-4E04-9AC5-8190C2D4310A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17081500" y="17119600"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>292100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3384719</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1231948</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0296C459-F8DE-42E6-8FA6-4DF639632596}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17056100" y="18592800"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>254000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3435519</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1193848</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF3B77F0-24FE-4430-8BD1-5550CC9664F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17106900" y="19964400"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3422819</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>1168448</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E98BB4D-0B00-45AF-95E7-D57B13E4039C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17094200" y="21412200"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3435519</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1117648</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1429C197-B837-441C-81E3-4EEC2DF5B972}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17106900" y="22783800"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3410119</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1206548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C50DFD10-6939-49D0-88E3-66028A939C3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17081500" y="24193500"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>254000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3460919</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1193848</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B23E01E2-28B3-4FF7-A1D4-E89AFDFB7A42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17132300" y="25577800"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3448219</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>1168448</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36F93E47-AC77-4A2D-A510-C4AE093FC10F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17119600" y="26885900"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3473619</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>1054148</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{499238E4-2BE3-4B91-A3A1-D8C30D904CE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17145000" y="28079700"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3448219</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>1219248</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E37159E2-F04B-4FED-AE1B-070819DEBFD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17119600" y="29489400"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3372019</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>1295448</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{447D26BB-7303-434E-82D3-5E6283395BEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17043400" y="31165800"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3346619</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>1117648</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AC64BF8-0100-494D-A2C2-28197BC28596}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17018000" y="32562800"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3473619</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>1117648</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{357A8762-4CAA-4B78-A163-FD7CD009EC6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17145000" y="33896300"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3473619</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1066848</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89B824DD-3205-45BF-B719-ECFB00559FAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17145000" y="35102800"/>
+          <a:ext cx="3283119" cy="939848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>116416</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>137583</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2497788</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>753565</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DB58ACD-4974-4DB0-BFC2-5ECD0A1465F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12107333" y="5101166"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>169334</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2550706</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>774732</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5205AA12-4909-4DE8-9AF8-1AD5DEA2A66F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12160251" y="6053667"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>137583</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2518955</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>742982</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEDE135C-D9BE-409E-A7AA-1287348EA1D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12128500" y="7048500"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>116416</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2497788</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>721815</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E94A6AE0-B39A-4F8D-8B20-A3CEE2A7A29B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12107333" y="7958666"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>116417</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>116417</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2497789</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>732399</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83156A7C-8DFF-45AC-A918-F0147E39B6B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12107334" y="8847667"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>105834</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>137584</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2487206</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>753566</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDF46202-630C-494A-9015-701B4D7E5E52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12096751" y="9768417"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>105833</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>105834</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2487205</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>721816</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCC131E-AB11-4356-BBC6-3A4F67F4C7A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12096750" y="10604501"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>148166</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>275167</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2529538</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>891149</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A40627C2-DE31-44E1-A429-483018DFBF08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12139083" y="11641667"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>306916</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2508372</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>922898</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91AD7EE5-14A2-4EE7-87DD-366201286BA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12647083" y="5270499"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>84667</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>433916</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2466039</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>1049898</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD0B42A3-1694-4294-B9A8-24E4478A9AC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12604750" y="6741583"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>116416</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>444500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2497788</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1060482</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B24E1A3-A8E0-4022-A219-A3EEA16D546E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12636499" y="8339667"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>328083</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2508372</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>944065</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{848D770D-C9B4-472D-B5F6-C4446CE5CFBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12647083" y="9641416"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>84667</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>486833</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2466039</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1102815</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74D2EE32-0FA0-4F03-833E-86A2287A9E48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12604750" y="11017250"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>105833</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>338667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2487205</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>954649</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19466AAC-34D6-4201-A8B5-CB93F983E3DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12625916" y="12562417"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>338667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2508372</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>954649</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5564C035-0D6D-46EA-86A2-E16531536027}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12647083" y="13885334"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>105833</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>317500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2487205</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>933482</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{771821F8-F513-4420-8575-8B8D496B0C6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12625916" y="15091833"/>
+          <a:ext cx="2381372" cy="615982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1858,8 +4386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45444446-31EB-4750-B7BF-FDEF1F4BF163}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView zoomScale="59" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -1869,7 +4397,7 @@
     <col min="3" max="3" width="82.453125" style="7" customWidth="1"/>
     <col min="4" max="4" width="46.1796875" style="7" customWidth="1"/>
     <col min="5" max="5" width="47" style="7" customWidth="1"/>
-    <col min="6" max="6" width="37.1796875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="62.26953125" style="7" customWidth="1"/>
     <col min="7" max="7" width="24.81640625" style="7" customWidth="1"/>
     <col min="8" max="8" width="30" style="7" customWidth="1"/>
     <col min="9" max="9" width="24.1796875" style="7" customWidth="1"/>
@@ -2832,38 +5360,38 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="16" spans="1:10" s="62" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="I16" s="54" t="s">
+    <row r="16" spans="1:10" s="61" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I16" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="J16" s="54"/>
+      <c r="J16" s="53"/>
     </row>
     <row r="17" spans="1:9" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="D17" s="59" t="s">
+      <c r="D17" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="60" t="s">
+      <c r="E17" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="60" t="s">
+      <c r="F17" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="60" t="s">
+      <c r="G17" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="60" t="s">
+      <c r="H17" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="60" t="s">
+      <c r="I17" s="59" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2883,9 +5411,7 @@
       <c r="E18" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="F18" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F18" s="39"/>
       <c r="G18" s="40" t="s">
         <v>156</v>
       </c>
@@ -2896,7 +5422,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="186.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="42" t="s">
         <v>8</v>
       </c>
@@ -2912,9 +5438,7 @@
       <c r="E19" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="F19" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F19" s="39"/>
       <c r="G19" s="40" t="s">
         <v>156</v>
       </c>
@@ -2925,7 +5449,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="151" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="42" t="s">
         <v>7</v>
       </c>
@@ -2941,9 +5465,7 @@
       <c r="E20" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="F20" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F20" s="39"/>
       <c r="G20" s="40" t="s">
         <v>156</v>
       </c>
@@ -2954,7 +5476,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="136" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="42" t="s">
         <v>6</v>
       </c>
@@ -2970,9 +5492,7 @@
       <c r="E21" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="F21" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F21" s="39"/>
       <c r="G21" s="40" t="s">
         <v>156</v>
       </c>
@@ -2983,7 +5503,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="154" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="42" t="s">
         <v>5</v>
       </c>
@@ -2999,9 +5519,7 @@
       <c r="E22" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="F22" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F22" s="39"/>
       <c r="G22" s="40" t="s">
         <v>156</v>
       </c>
@@ -3012,7 +5530,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="42" t="s">
         <v>4</v>
       </c>
@@ -3028,9 +5546,7 @@
       <c r="E23" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="F23" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F23" s="39"/>
       <c r="G23" s="40" t="s">
         <v>156</v>
       </c>
@@ -3041,7 +5557,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="133" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="42" t="s">
         <v>3</v>
       </c>
@@ -3057,9 +5573,7 @@
       <c r="E24" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="F24" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F24" s="39"/>
       <c r="G24" s="40" t="s">
         <v>156</v>
       </c>
@@ -3070,7 +5584,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="144" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="42" t="s">
         <v>52</v>
       </c>
@@ -3086,9 +5600,7 @@
       <c r="E25" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="F25" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F25" s="39"/>
       <c r="G25" s="40" t="s">
         <v>156</v>
       </c>
@@ -3099,7 +5611,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="42" t="s">
         <v>108</v>
       </c>
@@ -3115,9 +5627,7 @@
       <c r="E26" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="F26" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F26" s="39"/>
       <c r="G26" s="40" t="s">
         <v>156</v>
       </c>
@@ -3128,7 +5638,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="156" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="42" t="s">
         <v>175</v>
       </c>
@@ -3144,9 +5654,7 @@
       <c r="E27" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="F27" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F27" s="39"/>
       <c r="G27" s="40" t="s">
         <v>156</v>
       </c>
@@ -3157,7 +5665,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="153" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="42" t="s">
         <v>178</v>
       </c>
@@ -3173,9 +5681,7 @@
       <c r="E28" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="F28" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F28" s="39"/>
       <c r="G28" s="40" t="s">
         <v>156</v>
       </c>
@@ -3186,7 +5692,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="142.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="42" t="s">
         <v>182</v>
       </c>
@@ -3202,9 +5708,7 @@
       <c r="E29" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="F29" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F29" s="39"/>
       <c r="G29" s="40" t="s">
         <v>156</v>
       </c>
@@ -3215,7 +5719,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="155.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="42" t="s">
         <v>185</v>
       </c>
@@ -3231,9 +5735,7 @@
       <c r="E30" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="F30" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F30" s="39"/>
       <c r="G30" s="40" t="s">
         <v>156</v>
       </c>
@@ -3244,7 +5746,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="147" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="42" t="s">
         <v>187</v>
       </c>
@@ -3260,9 +5762,7 @@
       <c r="E31" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="F31" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F31" s="39"/>
       <c r="G31" s="40" t="s">
         <v>156</v>
       </c>
@@ -3273,7 +5773,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="122.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="42" t="s">
         <v>189</v>
       </c>
@@ -3289,9 +5789,7 @@
       <c r="E32" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="F32" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F32" s="39"/>
       <c r="G32" s="40" t="s">
         <v>156</v>
       </c>
@@ -3302,7 +5800,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="65.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" ht="140" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="42" t="s">
         <v>192</v>
       </c>
@@ -3318,9 +5816,7 @@
       <c r="E33" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="F33" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F33" s="39"/>
       <c r="G33" s="40" t="s">
         <v>156</v>
       </c>
@@ -3331,7 +5827,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="71.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:21" ht="147.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="42" t="s">
         <v>195</v>
       </c>
@@ -3347,9 +5843,7 @@
       <c r="E34" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="F34" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F34" s="39"/>
       <c r="G34" s="40" t="s">
         <v>156</v>
       </c>
@@ -3360,7 +5854,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:21" ht="127.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="42" t="s">
         <v>198</v>
       </c>
@@ -3376,9 +5870,7 @@
       <c r="E35" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="F35" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F35" s="39"/>
       <c r="G35" s="40" t="s">
         <v>156</v>
       </c>
@@ -3389,7 +5881,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" ht="128.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
         <v>200</v>
       </c>
@@ -3405,9 +5897,7 @@
       <c r="E36" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="F36" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F36" s="39"/>
       <c r="G36" s="40" t="s">
         <v>42</v>
       </c>
@@ -3418,7 +5908,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" ht="124" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="42" t="s">
         <v>204</v>
       </c>
@@ -3434,9 +5924,7 @@
       <c r="E37" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="F37" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F37" s="39"/>
       <c r="G37" s="40" t="s">
         <v>156</v>
       </c>
@@ -3447,7 +5935,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" ht="129.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="42" t="s">
         <v>207</v>
       </c>
@@ -3463,9 +5951,7 @@
       <c r="E38" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="F38" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="F38" s="39"/>
       <c r="G38" s="40" t="s">
         <v>42</v>
       </c>
@@ -3527,6 +6013,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3534,7 +6021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40065796-B3BB-4692-98D1-FC0F357ABC96}">
   <dimension ref="A1:AS37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="75" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="75" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -3809,52 +6296,52 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:45" s="62" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="53" t="s">
+    <row r="16" spans="1:45" s="61" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="51"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52" t="s">
+      <c r="H16" s="51"/>
+      <c r="I16" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="52"/>
-      <c r="K16" s="61"/>
-      <c r="AS16" s="63"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="60"/>
+      <c r="AS16" s="62"/>
     </row>
     <row r="17" spans="1:45" ht="45" x14ac:dyDescent="0.35">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="58" t="s">
+      <c r="F17" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="58" t="s">
+      <c r="G17" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="58" t="s">
+      <c r="H17" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="58" t="s">
+      <c r="I17" s="57" t="s">
         <v>10</v>
       </c>
       <c r="J17" s="7"/>
@@ -4182,8 +6669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC49CB18-A6E0-49A5-938B-B75CF66915AA}">
   <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView topLeftCell="A13" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7265625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4193,7 +6680,7 @@
     <col min="3" max="3" width="95.26953125" style="1" customWidth="1"/>
     <col min="4" max="4" width="38" style="1" customWidth="1"/>
     <col min="5" max="5" width="51.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="40.6328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="50.81640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="25.54296875" style="1" customWidth="1"/>
     <col min="8" max="8" width="30.54296875" style="1" customWidth="1"/>
     <col min="9" max="9" width="20.81640625" style="1" customWidth="1"/>
@@ -5346,38 +7833,38 @@
         <v>209</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="64"/>
-      <c r="I16" s="54" t="s">
+    <row r="16" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F16" s="63"/>
+      <c r="I16" s="53" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:20" s="27" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="D17" s="59" t="s">
+      <c r="D17" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="60" t="s">
+      <c r="E17" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="60" t="s">
+      <c r="F17" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="60" t="s">
+      <c r="G17" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="60" t="s">
+      <c r="H17" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="60" t="s">
+      <c r="I17" s="59" t="s">
         <v>10</v>
       </c>
       <c r="J17" s="7"/>
@@ -5386,7 +7873,7 @@
       <c r="S17" s="28"/>
       <c r="T17" s="28"/>
     </row>
-    <row r="18" spans="1:20" s="27" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" s="27" customFormat="1" ht="127" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="42" t="s">
         <v>9</v>
       </c>
@@ -5420,7 +7907,7 @@
       <c r="S18" s="28"/>
       <c r="T18" s="28"/>
     </row>
-    <row r="19" spans="1:20" s="27" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" s="27" customFormat="1" ht="137" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="42" t="s">
         <v>8</v>
       </c>
@@ -5436,9 +7923,7 @@
       <c r="E19" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="F19" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F19" s="39"/>
       <c r="G19" s="40" t="s">
         <v>2</v>
       </c>
@@ -5454,7 +7939,7 @@
       <c r="S19" s="28"/>
       <c r="T19" s="28"/>
     </row>
-    <row r="20" spans="1:20" s="27" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" s="27" customFormat="1" ht="122.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="42" t="s">
         <v>7</v>
       </c>
@@ -5470,9 +7955,7 @@
       <c r="E20" s="38" t="s">
         <v>217</v>
       </c>
-      <c r="F20" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F20" s="39"/>
       <c r="G20" s="40" t="s">
         <v>2</v>
       </c>
@@ -5488,7 +7971,7 @@
       <c r="S20" s="28"/>
       <c r="T20" s="28"/>
     </row>
-    <row r="21" spans="1:20" s="27" customFormat="1" ht="96.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" s="27" customFormat="1" ht="131.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="42" t="s">
         <v>6</v>
       </c>
@@ -5504,9 +7987,7 @@
       <c r="E21" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="F21" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F21" s="39"/>
       <c r="G21" s="40" t="s">
         <v>42</v>
       </c>
@@ -5522,7 +8003,7 @@
       <c r="S21" s="28"/>
       <c r="T21" s="28"/>
     </row>
-    <row r="22" spans="1:20" s="27" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" s="27" customFormat="1" ht="131" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="42" t="s">
         <v>5</v>
       </c>
@@ -5538,9 +8019,7 @@
       <c r="E22" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="F22" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F22" s="39"/>
       <c r="G22" s="40" t="s">
         <v>2</v>
       </c>
@@ -5556,7 +8035,7 @@
       <c r="S22" s="28"/>
       <c r="T22" s="28"/>
     </row>
-    <row r="23" spans="1:20" s="27" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" s="27" customFormat="1" ht="110" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="42" t="s">
         <v>4</v>
       </c>
@@ -5572,9 +8051,7 @@
       <c r="E23" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="F23" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F23" s="39"/>
       <c r="G23" s="40" t="s">
         <v>2</v>
       </c>
@@ -5606,9 +8083,7 @@
       <c r="E24" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="F24" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F24" s="39"/>
       <c r="G24" s="40" t="s">
         <v>2</v>
       </c>
@@ -5624,7 +8099,7 @@
       <c r="S24" s="28"/>
       <c r="T24" s="28"/>
     </row>
-    <row r="25" spans="1:20" s="27" customFormat="1" ht="122.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" s="27" customFormat="1" ht="134" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="42" t="s">
         <v>52</v>
       </c>
@@ -5640,9 +8115,7 @@
       <c r="E25" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="F25" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F25" s="39"/>
       <c r="G25" s="40" t="s">
         <v>2</v>
       </c>
@@ -5657,7 +8130,7 @@
       <c r="S25" s="28"/>
       <c r="T25" s="28"/>
     </row>
-    <row r="26" spans="1:20" ht="84" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" ht="124" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="42" t="s">
         <v>108</v>
       </c>
@@ -5673,9 +8146,7 @@
       <c r="E26" s="38" t="s">
         <v>234</v>
       </c>
-      <c r="F26" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F26" s="39"/>
       <c r="G26" s="40" t="s">
         <v>2</v>
       </c>
@@ -5686,7 +8157,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="74.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" ht="110.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="42" t="s">
         <v>175</v>
       </c>
@@ -5702,9 +8173,7 @@
       <c r="E27" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="F27" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F27" s="39"/>
       <c r="G27" s="40" t="s">
         <v>2</v>
       </c>
@@ -5715,7 +8184,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" ht="115.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="42" t="s">
         <v>178</v>
       </c>
@@ -5731,9 +8200,7 @@
       <c r="E28" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="F28" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F28" s="39"/>
       <c r="G28" s="40" t="s">
         <v>42</v>
       </c>
@@ -5744,7 +8211,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" ht="111.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="42" t="s">
         <v>182</v>
       </c>
@@ -5760,9 +8227,7 @@
       <c r="E29" s="38" t="s">
         <v>244</v>
       </c>
-      <c r="F29" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F29" s="39"/>
       <c r="G29" s="40" t="s">
         <v>2</v>
       </c>
@@ -5773,7 +8238,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" ht="104" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="42" t="s">
         <v>185</v>
       </c>
@@ -5789,9 +8254,7 @@
       <c r="E30" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="F30" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F30" s="39"/>
       <c r="G30" s="40" t="s">
         <v>2</v>
       </c>
@@ -5802,7 +8265,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" ht="109.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="42" t="s">
         <v>187</v>
       </c>
@@ -5818,9 +8281,7 @@
       <c r="E31" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="F31" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F31" s="39"/>
       <c r="G31" s="40" t="s">
         <v>2</v>
       </c>
@@ -5831,7 +8292,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" ht="104.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="42" t="s">
         <v>189</v>
       </c>
@@ -5847,9 +8308,7 @@
       <c r="E32" s="38" t="s">
         <v>252</v>
       </c>
-      <c r="F32" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F32" s="39"/>
       <c r="G32" s="40" t="s">
         <v>2</v>
       </c>
@@ -5860,7 +8319,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="103" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="42" t="s">
         <v>192</v>
       </c>
@@ -5876,9 +8335,7 @@
       <c r="E33" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="F33" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F33" s="39"/>
       <c r="G33" s="40" t="s">
         <v>2</v>
       </c>
@@ -5889,7 +8346,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="42" t="s">
         <v>195</v>
       </c>
@@ -5905,9 +8362,7 @@
       <c r="E34" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="F34" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F34" s="39"/>
       <c r="G34" s="40" t="s">
         <v>2</v>
       </c>
@@ -5918,7 +8373,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="126" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="42" t="s">
         <v>198</v>
       </c>
@@ -5934,9 +8389,7 @@
       <c r="E35" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="F35" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F35" s="39"/>
       <c r="G35" s="40" t="s">
         <v>2</v>
       </c>
@@ -5947,7 +8400,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" ht="124" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
         <v>200</v>
       </c>
@@ -5963,9 +8416,7 @@
       <c r="E36" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="F36" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F36" s="39"/>
       <c r="G36" s="40" t="s">
         <v>2</v>
       </c>
@@ -5976,7 +8427,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="105" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="42" t="s">
         <v>204</v>
       </c>
@@ -5992,9 +8443,7 @@
       <c r="E37" s="38" t="s">
         <v>264</v>
       </c>
-      <c r="F37" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F37" s="39"/>
       <c r="G37" s="40" t="s">
         <v>42</v>
       </c>
@@ -6005,7 +8454,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" ht="99" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="42" t="s">
         <v>207</v>
       </c>
@@ -6021,9 +8470,7 @@
       <c r="E38" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="F38" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F38" s="39"/>
       <c r="G38" s="40" t="s">
         <v>42</v>
       </c>
@@ -6034,7 +8481,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="104" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="42" t="s">
         <v>265</v>
       </c>
@@ -6050,9 +8497,7 @@
       <c r="E39" s="38" t="s">
         <v>244</v>
       </c>
-      <c r="F39" s="39" t="s">
-        <v>13</v>
-      </c>
+      <c r="F39" s="39"/>
       <c r="G39" s="40" t="s">
         <v>2</v>
       </c>
@@ -6086,6 +8531,7 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CSeite &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6093,8 +8539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8700AC-5695-489F-8EEA-6C3C9EFF921F}">
   <dimension ref="A1:AS37"/>
   <sheetViews>
-    <sheetView zoomScale="73" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView topLeftCell="A23" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -6104,7 +8550,7 @@
     <col min="3" max="3" width="34.7265625" style="23" customWidth="1"/>
     <col min="4" max="4" width="35.81640625" style="23" customWidth="1"/>
     <col min="5" max="5" width="49.90625" style="23" customWidth="1"/>
-    <col min="6" max="6" width="32.90625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="37.6328125" style="23" customWidth="1"/>
     <col min="7" max="7" width="19.453125" style="23" customWidth="1"/>
     <col min="8" max="8" width="31.81640625" style="23" customWidth="1"/>
     <col min="9" max="9" width="26.7265625" style="23" customWidth="1"/>
@@ -6366,52 +8812,52 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:45" s="62" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="53" t="s">
+    <row r="16" spans="1:45" s="61" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="51"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52" t="s">
+      <c r="H16" s="51"/>
+      <c r="I16" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="52"/>
-      <c r="K16" s="61"/>
-      <c r="AS16" s="63"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="60"/>
+      <c r="AS16" s="62"/>
     </row>
     <row r="17" spans="1:45" ht="45" x14ac:dyDescent="0.35">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="58" t="s">
+      <c r="F17" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="58" t="s">
+      <c r="G17" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="58" t="s">
+      <c r="H17" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="58" t="s">
+      <c r="I17" s="57" t="s">
         <v>10</v>
       </c>
       <c r="J17" s="7"/>
@@ -6460,9 +8906,7 @@
       <c r="E19" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F19" s="35"/>
       <c r="G19" s="9" t="s">
         <v>2</v>
       </c>
@@ -6488,9 +8932,7 @@
       <c r="E20" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F20" s="35"/>
       <c r="G20" s="9" t="s">
         <v>42</v>
       </c>
@@ -6516,9 +8958,7 @@
       <c r="E21" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F21" s="35"/>
       <c r="G21" s="9" t="s">
         <v>2</v>
       </c>
@@ -6544,9 +8984,7 @@
       <c r="E22" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="F22" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F22" s="35"/>
       <c r="G22" s="9" t="s">
         <v>2</v>
       </c>
@@ -6572,9 +9010,7 @@
       <c r="E23" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F23" s="35"/>
       <c r="G23" s="9" t="s">
         <v>2</v>
       </c>
@@ -6600,9 +9036,7 @@
       <c r="E24" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="F24" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F24" s="35"/>
       <c r="G24" s="9" t="s">
         <v>2</v>
       </c>
@@ -6628,9 +9062,7 @@
       <c r="E25" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="F25" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F25" s="35"/>
       <c r="G25" s="9" t="s">
         <v>2</v>
       </c>
@@ -6656,9 +9088,7 @@
       <c r="E26" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="F26" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F26" s="35"/>
       <c r="G26" s="9" t="s">
         <v>100</v>
       </c>
@@ -6720,6 +9150,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6727,8 +9158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DE9D5A-0BE0-43D3-BA55-9B3BEBABDE7D}">
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="101" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView topLeftCell="A25" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7265625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -6800,10 +9231,10 @@
       <c r="A8" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="64" t="s">
         <v>328</v>
       </c>
-      <c r="C8" s="51"/>
+      <c r="C8" s="64"/>
       <c r="D8" s="45"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
@@ -6814,44 +9245,44 @@
         <v>329</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="52" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="53" t="s">
+    <row r="16" spans="1:15" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F16" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="52" t="s">
+      <c r="I16" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="O16" s="54"/>
+      <c r="O16" s="53"/>
     </row>
     <row r="17" spans="1:20" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.35">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="58" t="s">
+      <c r="F17" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="58" t="s">
+      <c r="G17" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="58" t="s">
+      <c r="H17" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="58" t="s">
+      <c r="I17" s="57" t="s">
         <v>10</v>
       </c>
       <c r="J17" s="7"/>
@@ -6908,9 +9339,7 @@
       <c r="E19" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F19" s="35"/>
       <c r="G19" s="9" t="s">
         <v>2</v>
       </c>
@@ -6940,9 +9369,7 @@
       <c r="E20" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F20" s="35"/>
       <c r="G20" s="9" t="s">
         <v>42</v>
       </c>
@@ -6972,9 +9399,7 @@
       <c r="E21" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F21" s="35"/>
       <c r="G21" s="9" t="s">
         <v>2</v>
       </c>
@@ -7004,9 +9429,7 @@
       <c r="E22" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F22" s="35"/>
       <c r="G22" s="9" t="s">
         <v>2</v>
       </c>
@@ -7036,9 +9459,7 @@
       <c r="E23" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F23" s="35"/>
       <c r="G23" s="9" t="s">
         <v>2</v>
       </c>
@@ -7068,9 +9489,7 @@
       <c r="E24" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="F24" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F24" s="35"/>
       <c r="G24" s="9" t="s">
         <v>2</v>
       </c>
@@ -7100,9 +9519,7 @@
       <c r="E25" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="F25" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F25" s="35"/>
       <c r="G25" s="9" t="s">
         <v>2</v>
       </c>
@@ -7132,9 +9549,7 @@
       <c r="E26" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="F26" s="35" t="s">
-        <v>308</v>
-      </c>
+      <c r="F26" s="35"/>
       <c r="G26" s="9" t="s">
         <v>100</v>
       </c>
@@ -7173,6 +9588,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7180,7 +9596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D3C0FE-2E3C-45C0-A3A5-2800B3F6ED07}">
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView topLeftCell="G23" zoomScale="104" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -7252,10 +9668,10 @@
       <c r="A8" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="64" t="s">
         <v>330</v>
       </c>
-      <c r="C8" s="51"/>
+      <c r="C8" s="64"/>
       <c r="D8" s="45"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
@@ -7266,44 +9682,44 @@
         <v>331</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="52" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="53" t="s">
+    <row r="16" spans="1:15" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F16" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="52" t="s">
+      <c r="I16" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="O16" s="54"/>
+      <c r="O16" s="53"/>
     </row>
     <row r="17" spans="1:20" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.35">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="58" t="s">
+      <c r="F17" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="58" t="s">
+      <c r="G17" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="58" t="s">
+      <c r="H17" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="58" t="s">
+      <c r="I17" s="57" t="s">
         <v>10</v>
       </c>
       <c r="J17" s="7"/>
@@ -7656,10 +10072,10 @@
       <c r="A8" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="64" t="s">
         <v>332</v>
       </c>
-      <c r="C8" s="51"/>
+      <c r="C8" s="64"/>
       <c r="D8" s="45"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
@@ -7675,44 +10091,44 @@
         <v>334</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="52" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="53" t="s">
+    <row r="16" spans="1:15" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F16" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="52" t="s">
+      <c r="I16" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="O16" s="54"/>
+      <c r="O16" s="53"/>
     </row>
     <row r="17" spans="1:20" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.35">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="58" t="s">
+      <c r="F17" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="58" t="s">
+      <c r="G17" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="58" t="s">
+      <c r="H17" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="58" t="s">
+      <c r="I17" s="57" t="s">
         <v>10</v>
       </c>
       <c r="J17" s="7"/>
@@ -8055,10 +10471,10 @@
       <c r="A8" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="64" t="s">
         <v>336</v>
       </c>
-      <c r="C8" s="51"/>
+      <c r="C8" s="64"/>
       <c r="D8" s="45"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
@@ -8081,44 +10497,44 @@
         <v>338</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="52" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="53" t="s">
+    <row r="16" spans="1:15" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F16" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="52" t="s">
+      <c r="I16" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="O16" s="54"/>
+      <c r="O16" s="53"/>
     </row>
     <row r="17" spans="1:20" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.35">
-      <c r="A17" s="55" t="s">
+      <c r="A17" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="55" t="s">
+      <c r="D17" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="56" t="s">
+      <c r="F17" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="56" t="s">
+      <c r="G17" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="56" t="s">
+      <c r="H17" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="56" t="s">
+      <c r="I17" s="55" t="s">
         <v>10</v>
       </c>
       <c r="J17" s="7"/>
@@ -8796,10 +11212,10 @@
       <c r="A8" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="64" t="s">
         <v>268</v>
       </c>
-      <c r="C8" s="51"/>
+      <c r="C8" s="64"/>
       <c r="D8" s="45"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
@@ -8822,44 +11238,44 @@
         <v>339</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="52" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="53" t="s">
+    <row r="16" spans="1:15" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F16" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="52" t="s">
+      <c r="I16" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="O16" s="54"/>
+      <c r="O16" s="53"/>
     </row>
     <row r="17" spans="1:20" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.35">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="58" t="s">
+      <c r="F17" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="58" t="s">
+      <c r="G17" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="58" t="s">
+      <c r="H17" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="58" t="s">
+      <c r="I17" s="57" t="s">
         <v>10</v>
       </c>
       <c r="J17" s="7"/>
@@ -9679,52 +12095,52 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:45" s="62" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="53" t="s">
+    <row r="16" spans="1:45" s="61" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="51"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52" t="s">
+      <c r="H16" s="51"/>
+      <c r="I16" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="52"/>
-      <c r="K16" s="61"/>
-      <c r="AS16" s="63"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="60"/>
+      <c r="AS16" s="62"/>
     </row>
     <row r="17" spans="1:45" ht="45" x14ac:dyDescent="0.35">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="58" t="s">
+      <c r="F17" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="58" t="s">
+      <c r="G17" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="58" t="s">
+      <c r="H17" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="58" t="s">
+      <c r="I17" s="57" t="s">
         <v>10</v>
       </c>
       <c r="J17" s="7"/>

</xml_diff>